<commit_message>
update milestone from 18th/Nov/2017 view
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\userdata\q5894c\Desktop\6-group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MingjingLiu\ForMyself\GitHub\share\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8250" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="xubuju" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="shenivan" sheetId="19" r:id="rId4"/>
     <sheet name="xuzhihua" sheetId="20" r:id="rId5"/>
     <sheet name="liumingjing" sheetId="21" r:id="rId6"/>
+    <sheet name="milestone" sheetId="22" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="71">
   <si>
     <t>Task ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,6 +131,176 @@
     <t>TID12345_2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017/11/5~11/11</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/12~11/18</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/19~11/25</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/26~12/02</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/03~12/09</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/10~12/16</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/17~12/23</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/24~12~30</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/31~1/6</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/7~1/13</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/14~1/20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/21~1/27</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/28~2/3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/4~2/10</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>week</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>W45</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>W46</t>
+  </si>
+  <si>
+    <t>W47</t>
+  </si>
+  <si>
+    <t>W48</t>
+  </si>
+  <si>
+    <t>W49</t>
+  </si>
+  <si>
+    <t>W50</t>
+  </si>
+  <si>
+    <t>W51</t>
+  </si>
+  <si>
+    <t>W52</t>
+  </si>
+  <si>
+    <t>W01</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>W02</t>
+  </si>
+  <si>
+    <t>W03</t>
+  </si>
+  <si>
+    <t>W04</t>
+  </si>
+  <si>
+    <t>W05</t>
+  </si>
+  <si>
+    <t>W06</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>W07</t>
+  </si>
+  <si>
+    <t>W08</t>
+  </si>
+  <si>
+    <t>W09</t>
+  </si>
+  <si>
+    <t>product dev(Framework)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>study ThinkPHP</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>start to dev</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>60% complete</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>complete</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>product dev(Application)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>UML start</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>start to design website</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>must provide the data struct</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>system test</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>start</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company regestered</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>others</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +310,7 @@
     <numFmt numFmtId="176" formatCode="m/d;@"/>
     <numFmt numFmtId="177" formatCode="[$-804]aaa;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +358,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -302,6 +486,15 @@
     </xf>
     <xf numFmtId="176" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -620,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -84062,4 +84255,271 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="18">
+        <v>43159</v>
+      </c>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="28.5">
+      <c r="A3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+    </row>
+    <row r="4" spans="1:18" ht="28.5">
+      <c r="A4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+    </row>
+    <row r="6" spans="1:18" ht="28.5">
+      <c r="A6" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>